<commit_message>
PKA-1195 Create test to import from excel
</commit_message>
<xml_diff>
--- a/database/seeders/uploads/local/employees.xlsx
+++ b/database/seeders/uploads/local/employees.xlsx
@@ -15,96 +15,192 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Contact Name</t>
-  </si>
-  <si>
-    <t>Date of Birth</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+  <si>
+    <t>Worker Number</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Alias</t>
   </si>
   <si>
     <t>Job Title</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>icjo</t>
-  </si>
-  <si>
-    <t>Gillian Flatley</t>
-  </si>
-  <si>
-    <t>1999-11-05</t>
-  </si>
-  <si>
-    <t>Telecommunications Line Installer</t>
-  </si>
-  <si>
-    <t>camden.lebsack@gmail.com</t>
-  </si>
-  <si>
-    <t>bngw</t>
-  </si>
-  <si>
-    <t>Prof. Jordy Prosacco</t>
-  </si>
-  <si>
-    <t>2011-12-07</t>
-  </si>
-  <si>
-    <t>Engine Assembler</t>
-  </si>
-  <si>
-    <t>cormier.golden@gmail.com</t>
-  </si>
-  <si>
-    <t>jwww</t>
-  </si>
-  <si>
-    <t>Mr. Cordelia Tremblay</t>
-  </si>
-  <si>
-    <t>2021-01-21</t>
-  </si>
-  <si>
-    <t>Production Worker</t>
-  </si>
-  <si>
-    <t>kailey.bogisich@larson.biz</t>
-  </si>
-  <si>
-    <t>xlae</t>
-  </si>
-  <si>
-    <t>Cody Hayes</t>
-  </si>
-  <si>
-    <t>1973-05-05</t>
-  </si>
-  <si>
-    <t>Loan Interviewer</t>
-  </si>
-  <si>
-    <t>avis49@bins.biz</t>
-  </si>
-  <si>
-    <t>jhtp</t>
-  </si>
-  <si>
-    <t>Tyree Schmeler</t>
-  </si>
-  <si>
-    <t>2005-05-31</t>
-  </si>
-  <si>
-    <t>Algorithm Developer</t>
-  </si>
-  <si>
-    <t>syble.hartmann@pfeffer.com</t>
+    <t>Positions</t>
+  </si>
+  <si>
+    <t>Starting Date</t>
+  </si>
+  <si>
+    <t>Workplace</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>reset password</t>
+  </si>
+  <si>
+    <t>Aurelio Hintz Sr.</t>
+  </si>
+  <si>
+    <t>henderson.mosciski</t>
+  </si>
+  <si>
+    <t>Continuous Mining Machine Operator</t>
+  </si>
+  <si>
+    <t>dev-w</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>adelia27</t>
+  </si>
+  <si>
+    <t>ND6]$`fU"[z04%A~</t>
+  </si>
+  <si>
+    <t>Prof. Abner Pfeffer V</t>
+  </si>
+  <si>
+    <t>talia.lakin</t>
+  </si>
+  <si>
+    <t>Aircraft Launch and Recovery Officer</t>
+  </si>
+  <si>
+    <t>weissnat.pattie</t>
+  </si>
+  <si>
+    <t>TU(BKTE4b#fI(R\,</t>
+  </si>
+  <si>
+    <t>Jayce Yost</t>
+  </si>
+  <si>
+    <t>trantow.krista</t>
+  </si>
+  <si>
+    <t>Shoe Machine Operators</t>
+  </si>
+  <si>
+    <t>kelley16</t>
+  </si>
+  <si>
+    <t>+1|w4FU+;g*[R+x*</t>
+  </si>
+  <si>
+    <t>Judah Dickinson</t>
+  </si>
+  <si>
+    <t>ariel.hammes</t>
+  </si>
+  <si>
+    <t>Tank Car</t>
+  </si>
+  <si>
+    <t>nadia.kohler</t>
+  </si>
+  <si>
+    <t>d:LoJ@;H/w&lt;%$/{</t>
+  </si>
+  <si>
+    <t>Jackeline Brakus</t>
+  </si>
+  <si>
+    <t>dominic.murray</t>
+  </si>
+  <si>
+    <t>Anthropologist OR Archeologist</t>
+  </si>
+  <si>
+    <t>nettie13</t>
+  </si>
+  <si>
+    <t>NpACR32U,rL9"Q$DO)&gt;</t>
+  </si>
+  <si>
+    <t>Verna Kuphal III</t>
+  </si>
+  <si>
+    <t>haleigh24</t>
+  </si>
+  <si>
+    <t>Woodworking Machine Operator</t>
+  </si>
+  <si>
+    <t>jerrold.stamm</t>
+  </si>
+  <si>
+    <t>7~o73T</t>
+  </si>
+  <si>
+    <t>Prof. Torrance Streich PhD</t>
+  </si>
+  <si>
+    <t>aniyah47</t>
+  </si>
+  <si>
+    <t>Pile-Driver Operator</t>
+  </si>
+  <si>
+    <t>larue.jacobs</t>
+  </si>
+  <si>
+    <t>nAr?zzhmF3u9&gt;</t>
+  </si>
+  <si>
+    <t>Verla Baumbach</t>
+  </si>
+  <si>
+    <t>feeney.antonietta</t>
+  </si>
+  <si>
+    <t>Pharmacy Technician</t>
+  </si>
+  <si>
+    <t>towne.lorena</t>
+  </si>
+  <si>
+    <t>_)^@I,CK}-lCls</t>
+  </si>
+  <si>
+    <t>Ms. Keara Mayert V</t>
+  </si>
+  <si>
+    <t>kyle47</t>
+  </si>
+  <si>
+    <t>Chef</t>
+  </si>
+  <si>
+    <t>turcotte.jacinthe</t>
+  </si>
+  <si>
+    <t>Q}dN36.'_?7}.9g'=^X9</t>
+  </si>
+  <si>
+    <t>Jennifer Kuhic</t>
+  </si>
+  <si>
+    <t>nkuhlman</t>
+  </si>
+  <si>
+    <t>Distribution Manager</t>
+  </si>
+  <si>
+    <t>stehr.anissa</t>
+  </si>
+  <si>
+    <t>@#+{r`IJugO</t>
   </si>
 </sst>
 </file>
@@ -444,7 +540,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +548,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,90 +564,340 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>171</v>
+      </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>31877.0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>2559</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3">
+        <v>39033.0</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>15</v>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>2809</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>43465.0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>3704</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="F5">
+        <v>34697.0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>8528</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>42756.0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>9682</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <v>36987.0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>4149</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>37387.0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>8213</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>32550.0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>2227</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10">
+        <v>36293.0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>5664</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11">
+        <v>38410.0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>